<commit_message>
Add PracticeFormTests for validating form submissions; refactor PracticeFormPage to enhance form handling and data entry; introduce FormDataProvider for dynamic test data generation
</commit_message>
<xml_diff>
--- a/src/test/resources/test_sheet.xlsx
+++ b/src/test/resources/test_sheet.xlsx
@@ -8,22 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\code\Java_selenium\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47116798-CB14-4AE5-9708-128D908296D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A274DD37-A476-4DF6-BA1C-74A507F58A81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="{0}" sheetId="1" r:id="rId1"/>
     <sheet name="{1}" sheetId="2" r:id="rId2"/>
     <sheet name="{2}" sheetId="3" r:id="rId3"/>
     <sheet name="{3}" sheetId="4" r:id="rId4"/>
+    <sheet name="{4}" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="284">
   <si>
     <t>name1</t>
   </si>
@@ -494,6 +495,387 @@
   </si>
   <si>
     <t>Column[5] Department</t>
+  </si>
+  <si>
+    <t>Column[0] FirstName</t>
+  </si>
+  <si>
+    <t>Column[1] LastName</t>
+  </si>
+  <si>
+    <t>English</t>
+  </si>
+  <si>
+    <t>Chemistry</t>
+  </si>
+  <si>
+    <t>Computer Science</t>
+  </si>
+  <si>
+    <t>Commerce</t>
+  </si>
+  <si>
+    <t>Economics</t>
+  </si>
+  <si>
+    <t>Social Studies</t>
+  </si>
+  <si>
+    <t>Arts</t>
+  </si>
+  <si>
+    <t>History</t>
+  </si>
+  <si>
+    <t>Maths</t>
+  </si>
+  <si>
+    <t>Accounting</t>
+  </si>
+  <si>
+    <t>Physics</t>
+  </si>
+  <si>
+    <t>Biology</t>
+  </si>
+  <si>
+    <t>Hindi</t>
+  </si>
+  <si>
+    <t>Civics</t>
+  </si>
+  <si>
+    <t>James</t>
+  </si>
+  <si>
+    <t>Olivia</t>
+  </si>
+  <si>
+    <t>William</t>
+  </si>
+  <si>
+    <t>Emma</t>
+  </si>
+  <si>
+    <t>Noah</t>
+  </si>
+  <si>
+    <t>Ava</t>
+  </si>
+  <si>
+    <t>Liam</t>
+  </si>
+  <si>
+    <t>Sophia</t>
+  </si>
+  <si>
+    <t>Elijah</t>
+  </si>
+  <si>
+    <t>Isabella</t>
+  </si>
+  <si>
+    <t>Oliver</t>
+  </si>
+  <si>
+    <t>Charlotte</t>
+  </si>
+  <si>
+    <t>Lucas</t>
+  </si>
+  <si>
+    <t>Amelia</t>
+  </si>
+  <si>
+    <t>Mason</t>
+  </si>
+  <si>
+    <t>Harper</t>
+  </si>
+  <si>
+    <t>Ethan</t>
+  </si>
+  <si>
+    <t>Evelyn</t>
+  </si>
+  <si>
+    <t>Alexander</t>
+  </si>
+  <si>
+    <t>Abigail</t>
+  </si>
+  <si>
+    <t>Smith</t>
+  </si>
+  <si>
+    <t>Johnson</t>
+  </si>
+  <si>
+    <t>Williams</t>
+  </si>
+  <si>
+    <t>Brown</t>
+  </si>
+  <si>
+    <t>Jones</t>
+  </si>
+  <si>
+    <t>Garcia</t>
+  </si>
+  <si>
+    <t>Miller</t>
+  </si>
+  <si>
+    <t>Davis</t>
+  </si>
+  <si>
+    <t>Rodriguez</t>
+  </si>
+  <si>
+    <t>Martinez</t>
+  </si>
+  <si>
+    <t>Hernandez</t>
+  </si>
+  <si>
+    <t>Lopez</t>
+  </si>
+  <si>
+    <t>Wilson</t>
+  </si>
+  <si>
+    <t>Anderson</t>
+  </si>
+  <si>
+    <t>Thomas</t>
+  </si>
+  <si>
+    <t>Taylor</t>
+  </si>
+  <si>
+    <t>Moore</t>
+  </si>
+  <si>
+    <t>Jackson</t>
+  </si>
+  <si>
+    <t>Martin</t>
+  </si>
+  <si>
+    <t>Lee</t>
+  </si>
+  <si>
+    <t>Perez</t>
+  </si>
+  <si>
+    <t>Thompson</t>
+  </si>
+  <si>
+    <t>White</t>
+  </si>
+  <si>
+    <t>Harris</t>
+  </si>
+  <si>
+    <t>Sanchez</t>
+  </si>
+  <si>
+    <t>Clark</t>
+  </si>
+  <si>
+    <t>Ramirez</t>
+  </si>
+  <si>
+    <t>Lewis</t>
+  </si>
+  <si>
+    <t>Robinson</t>
+  </si>
+  <si>
+    <t>Walker</t>
+  </si>
+  <si>
+    <t>james.smith88@gmail.com</t>
+  </si>
+  <si>
+    <t>olivia.johnson95@yahoo.com</t>
+  </si>
+  <si>
+    <t>william.brown22@outlook.com</t>
+  </si>
+  <si>
+    <t>emma.williams87@hotmail.com</t>
+  </si>
+  <si>
+    <t>noah.davis1990@gmail.com</t>
+  </si>
+  <si>
+    <t>ava.miller24@protonmail.com</t>
+  </si>
+  <si>
+    <t>liam.garcia18@yahoo.com</t>
+  </si>
+  <si>
+    <t>sophia.rodriguez99@icloud.com</t>
+  </si>
+  <si>
+    <t>elijah.martinez77@gmail.com</t>
+  </si>
+  <si>
+    <t>isabella.wilson2023@outlook.com</t>
+  </si>
+  <si>
+    <t>oliver.thomas45@hotmail.com</t>
+  </si>
+  <si>
+    <t>charlotte.jones81@gmail.com</t>
+  </si>
+  <si>
+    <t>lucas.anderson56@yahoo.com</t>
+  </si>
+  <si>
+    <t>amelia.taylor92@protonmail.com</t>
+  </si>
+  <si>
+    <t>mason.moore33@gmail.com</t>
+  </si>
+  <si>
+    <t>harper.jackson70@outlook.com</t>
+  </si>
+  <si>
+    <t>ethan.white19@hotmail.com</t>
+  </si>
+  <si>
+    <t>evelyn.harris64@gmail.com</t>
+  </si>
+  <si>
+    <t>alexander.lee88@yahoo.com</t>
+  </si>
+  <si>
+    <t>abigail.martin2024@icloud.com</t>
+  </si>
+  <si>
+    <t>noah.perez57@gmail.com</t>
+  </si>
+  <si>
+    <t>emma.thompson91@outlook.com</t>
+  </si>
+  <si>
+    <t>james.clark44@hotmail.com</t>
+  </si>
+  <si>
+    <t>olivia.ramirez77@gmail.com</t>
+  </si>
+  <si>
+    <t>william.lewis23@yahoo.com</t>
+  </si>
+  <si>
+    <t>sophia.robinson99@protonmail.com</t>
+  </si>
+  <si>
+    <t>liam.walker2025@gmail.com</t>
+  </si>
+  <si>
+    <t>ava.sanchez66@outlook.com</t>
+  </si>
+  <si>
+    <t>elijah.hernandez81@hotmail.com</t>
+  </si>
+  <si>
+    <t>isabella.lopez55@gmail.com</t>
+  </si>
+  <si>
+    <t>oliver.brown73@yahoo.com</t>
+  </si>
+  <si>
+    <t>charlotte.smith2022@icloud.com</t>
+  </si>
+  <si>
+    <t>lucas.wilson47@gmail.com</t>
+  </si>
+  <si>
+    <t>amelia.johnson88@protonmail.com</t>
+  </si>
+  <si>
+    <t>mason.davis91@gmail.com</t>
+  </si>
+  <si>
+    <t>Column[2] Emails</t>
+  </si>
+  <si>
+    <t>Column[3] BirthYear</t>
+  </si>
+  <si>
+    <t>Column[4] BirthMonth</t>
+  </si>
+  <si>
+    <t>Column[5] BirthDay</t>
+  </si>
+  <si>
+    <t>Column[6] Subjects</t>
+  </si>
+  <si>
+    <t>Column[7] Current address</t>
+  </si>
+  <si>
+    <t>123 Main Street, Apt. 45, New York, NY 10001</t>
+  </si>
+  <si>
+    <t>742 Evergreen Terrace, Springfield, IL 62704</t>
+  </si>
+  <si>
+    <t>221B Baker Street, London, NW1 6XE, United Kingdom</t>
+  </si>
+  <si>
+    <t>1600 Pennsylvania Avenue NW, Washington, DC 20500</t>
+  </si>
+  <si>
+    <t>10 Downing Street, London, SW1A 2AA, UK</t>
+  </si>
+  <si>
+    <t>4567 Oak Lane, Apt 12B, Los Angeles, California 90210</t>
+  </si>
+  <si>
+    <t>789 Pine Road #5A, Toronto, ON M5V 2J1, Canada</t>
+  </si>
+  <si>
+    <t>Flat 3B, 123 High Street, Manchester M4 1AB, United Kingdom</t>
+  </si>
+  <si>
+    <t>12/34 Smith St, Unit 8, Sydney NSW 2000, Australia</t>
+  </si>
+  <si>
+    <t>99 Rue de Rivoli, 75001 Paris, France</t>
+  </si>
+  <si>
+    <t>1 Infinite Loop, Cupertino, CA 95014</t>
+  </si>
+  <si>
+    <t>350 Fifth Avenue, Suite 1515, New York, NY 10118</t>
+  </si>
+  <si>
+    <t>P.O. Box 1234, Miami, FL 33131</t>
+  </si>
+  <si>
+    <t>45-67 Queens Boulevard, Apt 2C, Queens, NY 11101</t>
+  </si>
+  <si>
+    <t>1234½ Maple Drive, Beverly Hills, CA 90210</t>
+  </si>
+  <si>
+    <t>9876 Forest Hill Dr., Building C, Suite 300, Austin, TX 78701</t>
+  </si>
+  <si>
+    <t>555 Mission Street, Floor 12, San Francisco, CA 94105</t>
+  </si>
+  <si>
+    <t>7th Avenue &amp; West 34th Street, New York, NY 10001 (no house number)</t>
+  </si>
+  <si>
+    <t>42 Wallaby Way, Sydney, Australia</t>
+  </si>
+  <si>
+    <t>12345 Super Long Street Name That Keeps Going and Going, Apartment 999, Extremely Long City Name, California 98765-4321, United States of America</t>
   </si>
 </sst>
 </file>
@@ -571,7 +953,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
@@ -582,6 +964,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
@@ -803,7 +1186,7 @@
   </sheetPr>
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
@@ -1554,4 +1937,520 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{885B92C7-3673-4132-A4FB-24C9D0434248}">
+  <dimension ref="A1:H36"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="63" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>258</v>
+      </c>
+      <c r="D1" t="s">
+        <v>259</v>
+      </c>
+      <c r="E1" t="s">
+        <v>260</v>
+      </c>
+      <c r="F1" t="s">
+        <v>261</v>
+      </c>
+      <c r="G1" t="s">
+        <v>262</v>
+      </c>
+      <c r="H1" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="G2" t="s">
+        <v>159</v>
+      </c>
+      <c r="H2" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="H3" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="H4" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="H5" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="H6" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="H7" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="H8" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="H9" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="H10" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="H11" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="H12" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="H13" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="H14" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="H15" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="H16" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="H17" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="H18" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="H19" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="H20" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="H21" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B22" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B23" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B24" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B25" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B26" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B27" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B28" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B29" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B30" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B31" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C32" s="2" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="33" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C33" s="2" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="34" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C34" s="2" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="35" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C35" s="2" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="36" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C36" s="2" t="s">
+        <v>257</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" display="mailto:james.smith88@gmail.com" xr:uid="{116A487D-1019-4524-A7FE-CD987F51F4F6}"/>
+    <hyperlink ref="C3" r:id="rId2" display="mailto:olivia.johnson95@yahoo.com" xr:uid="{30B12E3A-BA70-41FE-9AB9-30A38FC4568A}"/>
+    <hyperlink ref="C4" r:id="rId3" display="mailto:william.brown22@outlook.com" xr:uid="{E6A6F286-45EB-431E-8F39-E57764F85827}"/>
+    <hyperlink ref="C5" r:id="rId4" display="mailto:emma.williams87@hotmail.com" xr:uid="{67B125E0-5B58-4A96-A085-0345DBE9E0C6}"/>
+    <hyperlink ref="C6" r:id="rId5" display="mailto:noah.davis1990@gmail.com" xr:uid="{47BC22A1-BABD-45C7-98F0-8EE68DC9B556}"/>
+    <hyperlink ref="C7" r:id="rId6" display="mailto:ava.miller24@protonmail.com" xr:uid="{A8C0E64A-2CD6-4B92-A935-5A269BE1D057}"/>
+    <hyperlink ref="C8" r:id="rId7" display="mailto:liam.garcia18@yahoo.com" xr:uid="{08C5A6B9-AB76-40CB-A3D0-57E4912D6356}"/>
+    <hyperlink ref="C9" r:id="rId8" display="mailto:sophia.rodriguez99@icloud.com" xr:uid="{548F8884-D276-4F31-820E-854C3A7FC83F}"/>
+    <hyperlink ref="C10" r:id="rId9" display="mailto:elijah.martinez77@gmail.com" xr:uid="{3F936122-D206-4BF7-BAA5-F6E27595F561}"/>
+    <hyperlink ref="C11" r:id="rId10" display="mailto:isabella.wilson2023@outlook.com" xr:uid="{849105D7-CE77-4F58-ABE3-5B3C38CF69D0}"/>
+    <hyperlink ref="C12" r:id="rId11" display="mailto:oliver.thomas45@hotmail.com" xr:uid="{AC85A189-3B5B-4051-A412-E0AA13EABF05}"/>
+    <hyperlink ref="C13" r:id="rId12" display="mailto:charlotte.jones81@gmail.com" xr:uid="{3F0393A3-0332-4867-AE14-089D18AA01DD}"/>
+    <hyperlink ref="C14" r:id="rId13" display="mailto:lucas.anderson56@yahoo.com" xr:uid="{1D41D4A1-C5C0-434F-BD71-A1EE7D0F9FDE}"/>
+    <hyperlink ref="C15" r:id="rId14" display="mailto:amelia.taylor92@protonmail.com" xr:uid="{91424D86-BCCF-4E47-96D7-FF9DD4C33374}"/>
+    <hyperlink ref="C16" r:id="rId15" display="mailto:mason.moore33@gmail.com" xr:uid="{11D2BB07-580B-4DFF-BBED-D388430927D4}"/>
+    <hyperlink ref="C17" r:id="rId16" display="mailto:harper.jackson70@outlook.com" xr:uid="{E3B41151-1586-49F0-BA0E-9498A32768D4}"/>
+    <hyperlink ref="C18" r:id="rId17" display="mailto:ethan.white19@hotmail.com" xr:uid="{D63BB15F-0BCE-4C71-954E-73A8A71D562D}"/>
+    <hyperlink ref="C19" r:id="rId18" display="mailto:evelyn.harris64@gmail.com" xr:uid="{927568C2-31CD-4A22-9CBC-B6793A63590D}"/>
+    <hyperlink ref="C20" r:id="rId19" display="mailto:alexander.lee88@yahoo.com" xr:uid="{3EA0F367-A587-41EA-911B-DA9814415F9A}"/>
+    <hyperlink ref="C21" r:id="rId20" display="mailto:abigail.martin2024@icloud.com" xr:uid="{94509102-8B04-4C0A-ACDC-4239CF1F9C53}"/>
+    <hyperlink ref="C22" r:id="rId21" display="mailto:noah.perez57@gmail.com" xr:uid="{AC8DFACE-88B6-4957-B3E0-F2C3297CA4B8}"/>
+    <hyperlink ref="C23" r:id="rId22" display="mailto:emma.thompson91@outlook.com" xr:uid="{BDE5FB59-7917-43DB-A0DC-2613E9982A53}"/>
+    <hyperlink ref="C24" r:id="rId23" display="mailto:james.clark44@hotmail.com" xr:uid="{4585C4FB-B906-4698-B0D6-9AEF4F50DE11}"/>
+    <hyperlink ref="C25" r:id="rId24" display="mailto:olivia.ramirez77@gmail.com" xr:uid="{EC90AA23-A0FC-401F-B433-0B6F434D2FFC}"/>
+    <hyperlink ref="C26" r:id="rId25" display="mailto:william.lewis23@yahoo.com" xr:uid="{660C0FD1-DDF9-4CDE-8A56-E14D82F699CF}"/>
+    <hyperlink ref="C27" r:id="rId26" display="mailto:sophia.robinson99@protonmail.com" xr:uid="{3C7DDDE7-1965-4C2B-9E74-F77BC199C081}"/>
+    <hyperlink ref="C28" r:id="rId27" display="mailto:liam.walker2025@gmail.com" xr:uid="{16C87169-6B6E-4262-A327-C844DA0C0D36}"/>
+    <hyperlink ref="C29" r:id="rId28" display="mailto:ava.sanchez66@outlook.com" xr:uid="{C2353843-FFE5-4283-A4D1-38F8AB5D6154}"/>
+    <hyperlink ref="C30" r:id="rId29" display="mailto:elijah.hernandez81@hotmail.com" xr:uid="{DF58218C-179D-488E-ABC6-E0B093A36D32}"/>
+    <hyperlink ref="C31" r:id="rId30" display="mailto:isabella.lopez55@gmail.com" xr:uid="{6419FB81-E30D-444A-B37B-FDAFA885B488}"/>
+    <hyperlink ref="C32" r:id="rId31" display="mailto:oliver.brown73@yahoo.com" xr:uid="{8DD94B64-DFD9-4C4E-B50A-EE6916960D04}"/>
+    <hyperlink ref="C33" r:id="rId32" display="mailto:charlotte.smith2022@icloud.com" xr:uid="{241A1B8E-E2DE-43A4-A595-764667291BC0}"/>
+    <hyperlink ref="C34" r:id="rId33" display="mailto:lucas.wilson47@gmail.com" xr:uid="{AB26F06E-9C46-4A44-AC32-4ED0C2CF8BC4}"/>
+    <hyperlink ref="C35" r:id="rId34" display="mailto:amelia.johnson88@protonmail.com" xr:uid="{4EA6D74B-6612-425B-960B-5C61FC15E2E6}"/>
+    <hyperlink ref="C36" r:id="rId35" display="mailto:mason.davis91@gmail.com" xr:uid="{C67E91C9-EAF1-4613-B55E-EB1BA772FEE7}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add PracticeFormTests for validating form submissions; refactor PracticeFormPage to enhance form handling and data entry; introduce FormDataProvider for dynamic test data generation (#40)
</commit_message>
<xml_diff>
--- a/src/test/resources/test_sheet.xlsx
+++ b/src/test/resources/test_sheet.xlsx
@@ -8,22 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\code\Java_selenium\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47116798-CB14-4AE5-9708-128D908296D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A274DD37-A476-4DF6-BA1C-74A507F58A81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="{0}" sheetId="1" r:id="rId1"/>
     <sheet name="{1}" sheetId="2" r:id="rId2"/>
     <sheet name="{2}" sheetId="3" r:id="rId3"/>
     <sheet name="{3}" sheetId="4" r:id="rId4"/>
+    <sheet name="{4}" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="284">
   <si>
     <t>name1</t>
   </si>
@@ -494,6 +495,387 @@
   </si>
   <si>
     <t>Column[5] Department</t>
+  </si>
+  <si>
+    <t>Column[0] FirstName</t>
+  </si>
+  <si>
+    <t>Column[1] LastName</t>
+  </si>
+  <si>
+    <t>English</t>
+  </si>
+  <si>
+    <t>Chemistry</t>
+  </si>
+  <si>
+    <t>Computer Science</t>
+  </si>
+  <si>
+    <t>Commerce</t>
+  </si>
+  <si>
+    <t>Economics</t>
+  </si>
+  <si>
+    <t>Social Studies</t>
+  </si>
+  <si>
+    <t>Arts</t>
+  </si>
+  <si>
+    <t>History</t>
+  </si>
+  <si>
+    <t>Maths</t>
+  </si>
+  <si>
+    <t>Accounting</t>
+  </si>
+  <si>
+    <t>Physics</t>
+  </si>
+  <si>
+    <t>Biology</t>
+  </si>
+  <si>
+    <t>Hindi</t>
+  </si>
+  <si>
+    <t>Civics</t>
+  </si>
+  <si>
+    <t>James</t>
+  </si>
+  <si>
+    <t>Olivia</t>
+  </si>
+  <si>
+    <t>William</t>
+  </si>
+  <si>
+    <t>Emma</t>
+  </si>
+  <si>
+    <t>Noah</t>
+  </si>
+  <si>
+    <t>Ava</t>
+  </si>
+  <si>
+    <t>Liam</t>
+  </si>
+  <si>
+    <t>Sophia</t>
+  </si>
+  <si>
+    <t>Elijah</t>
+  </si>
+  <si>
+    <t>Isabella</t>
+  </si>
+  <si>
+    <t>Oliver</t>
+  </si>
+  <si>
+    <t>Charlotte</t>
+  </si>
+  <si>
+    <t>Lucas</t>
+  </si>
+  <si>
+    <t>Amelia</t>
+  </si>
+  <si>
+    <t>Mason</t>
+  </si>
+  <si>
+    <t>Harper</t>
+  </si>
+  <si>
+    <t>Ethan</t>
+  </si>
+  <si>
+    <t>Evelyn</t>
+  </si>
+  <si>
+    <t>Alexander</t>
+  </si>
+  <si>
+    <t>Abigail</t>
+  </si>
+  <si>
+    <t>Smith</t>
+  </si>
+  <si>
+    <t>Johnson</t>
+  </si>
+  <si>
+    <t>Williams</t>
+  </si>
+  <si>
+    <t>Brown</t>
+  </si>
+  <si>
+    <t>Jones</t>
+  </si>
+  <si>
+    <t>Garcia</t>
+  </si>
+  <si>
+    <t>Miller</t>
+  </si>
+  <si>
+    <t>Davis</t>
+  </si>
+  <si>
+    <t>Rodriguez</t>
+  </si>
+  <si>
+    <t>Martinez</t>
+  </si>
+  <si>
+    <t>Hernandez</t>
+  </si>
+  <si>
+    <t>Lopez</t>
+  </si>
+  <si>
+    <t>Wilson</t>
+  </si>
+  <si>
+    <t>Anderson</t>
+  </si>
+  <si>
+    <t>Thomas</t>
+  </si>
+  <si>
+    <t>Taylor</t>
+  </si>
+  <si>
+    <t>Moore</t>
+  </si>
+  <si>
+    <t>Jackson</t>
+  </si>
+  <si>
+    <t>Martin</t>
+  </si>
+  <si>
+    <t>Lee</t>
+  </si>
+  <si>
+    <t>Perez</t>
+  </si>
+  <si>
+    <t>Thompson</t>
+  </si>
+  <si>
+    <t>White</t>
+  </si>
+  <si>
+    <t>Harris</t>
+  </si>
+  <si>
+    <t>Sanchez</t>
+  </si>
+  <si>
+    <t>Clark</t>
+  </si>
+  <si>
+    <t>Ramirez</t>
+  </si>
+  <si>
+    <t>Lewis</t>
+  </si>
+  <si>
+    <t>Robinson</t>
+  </si>
+  <si>
+    <t>Walker</t>
+  </si>
+  <si>
+    <t>james.smith88@gmail.com</t>
+  </si>
+  <si>
+    <t>olivia.johnson95@yahoo.com</t>
+  </si>
+  <si>
+    <t>william.brown22@outlook.com</t>
+  </si>
+  <si>
+    <t>emma.williams87@hotmail.com</t>
+  </si>
+  <si>
+    <t>noah.davis1990@gmail.com</t>
+  </si>
+  <si>
+    <t>ava.miller24@protonmail.com</t>
+  </si>
+  <si>
+    <t>liam.garcia18@yahoo.com</t>
+  </si>
+  <si>
+    <t>sophia.rodriguez99@icloud.com</t>
+  </si>
+  <si>
+    <t>elijah.martinez77@gmail.com</t>
+  </si>
+  <si>
+    <t>isabella.wilson2023@outlook.com</t>
+  </si>
+  <si>
+    <t>oliver.thomas45@hotmail.com</t>
+  </si>
+  <si>
+    <t>charlotte.jones81@gmail.com</t>
+  </si>
+  <si>
+    <t>lucas.anderson56@yahoo.com</t>
+  </si>
+  <si>
+    <t>amelia.taylor92@protonmail.com</t>
+  </si>
+  <si>
+    <t>mason.moore33@gmail.com</t>
+  </si>
+  <si>
+    <t>harper.jackson70@outlook.com</t>
+  </si>
+  <si>
+    <t>ethan.white19@hotmail.com</t>
+  </si>
+  <si>
+    <t>evelyn.harris64@gmail.com</t>
+  </si>
+  <si>
+    <t>alexander.lee88@yahoo.com</t>
+  </si>
+  <si>
+    <t>abigail.martin2024@icloud.com</t>
+  </si>
+  <si>
+    <t>noah.perez57@gmail.com</t>
+  </si>
+  <si>
+    <t>emma.thompson91@outlook.com</t>
+  </si>
+  <si>
+    <t>james.clark44@hotmail.com</t>
+  </si>
+  <si>
+    <t>olivia.ramirez77@gmail.com</t>
+  </si>
+  <si>
+    <t>william.lewis23@yahoo.com</t>
+  </si>
+  <si>
+    <t>sophia.robinson99@protonmail.com</t>
+  </si>
+  <si>
+    <t>liam.walker2025@gmail.com</t>
+  </si>
+  <si>
+    <t>ava.sanchez66@outlook.com</t>
+  </si>
+  <si>
+    <t>elijah.hernandez81@hotmail.com</t>
+  </si>
+  <si>
+    <t>isabella.lopez55@gmail.com</t>
+  </si>
+  <si>
+    <t>oliver.brown73@yahoo.com</t>
+  </si>
+  <si>
+    <t>charlotte.smith2022@icloud.com</t>
+  </si>
+  <si>
+    <t>lucas.wilson47@gmail.com</t>
+  </si>
+  <si>
+    <t>amelia.johnson88@protonmail.com</t>
+  </si>
+  <si>
+    <t>mason.davis91@gmail.com</t>
+  </si>
+  <si>
+    <t>Column[2] Emails</t>
+  </si>
+  <si>
+    <t>Column[3] BirthYear</t>
+  </si>
+  <si>
+    <t>Column[4] BirthMonth</t>
+  </si>
+  <si>
+    <t>Column[5] BirthDay</t>
+  </si>
+  <si>
+    <t>Column[6] Subjects</t>
+  </si>
+  <si>
+    <t>Column[7] Current address</t>
+  </si>
+  <si>
+    <t>123 Main Street, Apt. 45, New York, NY 10001</t>
+  </si>
+  <si>
+    <t>742 Evergreen Terrace, Springfield, IL 62704</t>
+  </si>
+  <si>
+    <t>221B Baker Street, London, NW1 6XE, United Kingdom</t>
+  </si>
+  <si>
+    <t>1600 Pennsylvania Avenue NW, Washington, DC 20500</t>
+  </si>
+  <si>
+    <t>10 Downing Street, London, SW1A 2AA, UK</t>
+  </si>
+  <si>
+    <t>4567 Oak Lane, Apt 12B, Los Angeles, California 90210</t>
+  </si>
+  <si>
+    <t>789 Pine Road #5A, Toronto, ON M5V 2J1, Canada</t>
+  </si>
+  <si>
+    <t>Flat 3B, 123 High Street, Manchester M4 1AB, United Kingdom</t>
+  </si>
+  <si>
+    <t>12/34 Smith St, Unit 8, Sydney NSW 2000, Australia</t>
+  </si>
+  <si>
+    <t>99 Rue de Rivoli, 75001 Paris, France</t>
+  </si>
+  <si>
+    <t>1 Infinite Loop, Cupertino, CA 95014</t>
+  </si>
+  <si>
+    <t>350 Fifth Avenue, Suite 1515, New York, NY 10118</t>
+  </si>
+  <si>
+    <t>P.O. Box 1234, Miami, FL 33131</t>
+  </si>
+  <si>
+    <t>45-67 Queens Boulevard, Apt 2C, Queens, NY 11101</t>
+  </si>
+  <si>
+    <t>1234½ Maple Drive, Beverly Hills, CA 90210</t>
+  </si>
+  <si>
+    <t>9876 Forest Hill Dr., Building C, Suite 300, Austin, TX 78701</t>
+  </si>
+  <si>
+    <t>555 Mission Street, Floor 12, San Francisco, CA 94105</t>
+  </si>
+  <si>
+    <t>7th Avenue &amp; West 34th Street, New York, NY 10001 (no house number)</t>
+  </si>
+  <si>
+    <t>42 Wallaby Way, Sydney, Australia</t>
+  </si>
+  <si>
+    <t>12345 Super Long Street Name That Keeps Going and Going, Apartment 999, Extremely Long City Name, California 98765-4321, United States of America</t>
   </si>
 </sst>
 </file>
@@ -571,7 +953,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
@@ -582,6 +964,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
@@ -803,7 +1186,7 @@
   </sheetPr>
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
@@ -1554,4 +1937,520 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{885B92C7-3673-4132-A4FB-24C9D0434248}">
+  <dimension ref="A1:H36"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="63" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>258</v>
+      </c>
+      <c r="D1" t="s">
+        <v>259</v>
+      </c>
+      <c r="E1" t="s">
+        <v>260</v>
+      </c>
+      <c r="F1" t="s">
+        <v>261</v>
+      </c>
+      <c r="G1" t="s">
+        <v>262</v>
+      </c>
+      <c r="H1" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="G2" t="s">
+        <v>159</v>
+      </c>
+      <c r="H2" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="H3" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="H4" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="H5" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="H6" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="H7" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="H8" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="H9" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="H10" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="H11" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="H12" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="H13" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="H14" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="H15" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="H16" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="H17" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="H18" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="H19" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="H20" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="H21" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B22" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B23" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B24" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B25" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B26" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B27" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B28" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B29" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B30" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B31" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C32" s="2" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="33" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C33" s="2" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="34" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C34" s="2" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="35" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C35" s="2" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="36" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C36" s="2" t="s">
+        <v>257</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" display="mailto:james.smith88@gmail.com" xr:uid="{116A487D-1019-4524-A7FE-CD987F51F4F6}"/>
+    <hyperlink ref="C3" r:id="rId2" display="mailto:olivia.johnson95@yahoo.com" xr:uid="{30B12E3A-BA70-41FE-9AB9-30A38FC4568A}"/>
+    <hyperlink ref="C4" r:id="rId3" display="mailto:william.brown22@outlook.com" xr:uid="{E6A6F286-45EB-431E-8F39-E57764F85827}"/>
+    <hyperlink ref="C5" r:id="rId4" display="mailto:emma.williams87@hotmail.com" xr:uid="{67B125E0-5B58-4A96-A085-0345DBE9E0C6}"/>
+    <hyperlink ref="C6" r:id="rId5" display="mailto:noah.davis1990@gmail.com" xr:uid="{47BC22A1-BABD-45C7-98F0-8EE68DC9B556}"/>
+    <hyperlink ref="C7" r:id="rId6" display="mailto:ava.miller24@protonmail.com" xr:uid="{A8C0E64A-2CD6-4B92-A935-5A269BE1D057}"/>
+    <hyperlink ref="C8" r:id="rId7" display="mailto:liam.garcia18@yahoo.com" xr:uid="{08C5A6B9-AB76-40CB-A3D0-57E4912D6356}"/>
+    <hyperlink ref="C9" r:id="rId8" display="mailto:sophia.rodriguez99@icloud.com" xr:uid="{548F8884-D276-4F31-820E-854C3A7FC83F}"/>
+    <hyperlink ref="C10" r:id="rId9" display="mailto:elijah.martinez77@gmail.com" xr:uid="{3F936122-D206-4BF7-BAA5-F6E27595F561}"/>
+    <hyperlink ref="C11" r:id="rId10" display="mailto:isabella.wilson2023@outlook.com" xr:uid="{849105D7-CE77-4F58-ABE3-5B3C38CF69D0}"/>
+    <hyperlink ref="C12" r:id="rId11" display="mailto:oliver.thomas45@hotmail.com" xr:uid="{AC85A189-3B5B-4051-A412-E0AA13EABF05}"/>
+    <hyperlink ref="C13" r:id="rId12" display="mailto:charlotte.jones81@gmail.com" xr:uid="{3F0393A3-0332-4867-AE14-089D18AA01DD}"/>
+    <hyperlink ref="C14" r:id="rId13" display="mailto:lucas.anderson56@yahoo.com" xr:uid="{1D41D4A1-C5C0-434F-BD71-A1EE7D0F9FDE}"/>
+    <hyperlink ref="C15" r:id="rId14" display="mailto:amelia.taylor92@protonmail.com" xr:uid="{91424D86-BCCF-4E47-96D7-FF9DD4C33374}"/>
+    <hyperlink ref="C16" r:id="rId15" display="mailto:mason.moore33@gmail.com" xr:uid="{11D2BB07-580B-4DFF-BBED-D388430927D4}"/>
+    <hyperlink ref="C17" r:id="rId16" display="mailto:harper.jackson70@outlook.com" xr:uid="{E3B41151-1586-49F0-BA0E-9498A32768D4}"/>
+    <hyperlink ref="C18" r:id="rId17" display="mailto:ethan.white19@hotmail.com" xr:uid="{D63BB15F-0BCE-4C71-954E-73A8A71D562D}"/>
+    <hyperlink ref="C19" r:id="rId18" display="mailto:evelyn.harris64@gmail.com" xr:uid="{927568C2-31CD-4A22-9CBC-B6793A63590D}"/>
+    <hyperlink ref="C20" r:id="rId19" display="mailto:alexander.lee88@yahoo.com" xr:uid="{3EA0F367-A587-41EA-911B-DA9814415F9A}"/>
+    <hyperlink ref="C21" r:id="rId20" display="mailto:abigail.martin2024@icloud.com" xr:uid="{94509102-8B04-4C0A-ACDC-4239CF1F9C53}"/>
+    <hyperlink ref="C22" r:id="rId21" display="mailto:noah.perez57@gmail.com" xr:uid="{AC8DFACE-88B6-4957-B3E0-F2C3297CA4B8}"/>
+    <hyperlink ref="C23" r:id="rId22" display="mailto:emma.thompson91@outlook.com" xr:uid="{BDE5FB59-7917-43DB-A0DC-2613E9982A53}"/>
+    <hyperlink ref="C24" r:id="rId23" display="mailto:james.clark44@hotmail.com" xr:uid="{4585C4FB-B906-4698-B0D6-9AEF4F50DE11}"/>
+    <hyperlink ref="C25" r:id="rId24" display="mailto:olivia.ramirez77@gmail.com" xr:uid="{EC90AA23-A0FC-401F-B433-0B6F434D2FFC}"/>
+    <hyperlink ref="C26" r:id="rId25" display="mailto:william.lewis23@yahoo.com" xr:uid="{660C0FD1-DDF9-4CDE-8A56-E14D82F699CF}"/>
+    <hyperlink ref="C27" r:id="rId26" display="mailto:sophia.robinson99@protonmail.com" xr:uid="{3C7DDDE7-1965-4C2B-9E74-F77BC199C081}"/>
+    <hyperlink ref="C28" r:id="rId27" display="mailto:liam.walker2025@gmail.com" xr:uid="{16C87169-6B6E-4262-A327-C844DA0C0D36}"/>
+    <hyperlink ref="C29" r:id="rId28" display="mailto:ava.sanchez66@outlook.com" xr:uid="{C2353843-FFE5-4283-A4D1-38F8AB5D6154}"/>
+    <hyperlink ref="C30" r:id="rId29" display="mailto:elijah.hernandez81@hotmail.com" xr:uid="{DF58218C-179D-488E-ABC6-E0B093A36D32}"/>
+    <hyperlink ref="C31" r:id="rId30" display="mailto:isabella.lopez55@gmail.com" xr:uid="{6419FB81-E30D-444A-B37B-FDAFA885B488}"/>
+    <hyperlink ref="C32" r:id="rId31" display="mailto:oliver.brown73@yahoo.com" xr:uid="{8DD94B64-DFD9-4C4E-B50A-EE6916960D04}"/>
+    <hyperlink ref="C33" r:id="rId32" display="mailto:charlotte.smith2022@icloud.com" xr:uid="{241A1B8E-E2DE-43A4-A595-764667291BC0}"/>
+    <hyperlink ref="C34" r:id="rId33" display="mailto:lucas.wilson47@gmail.com" xr:uid="{AB26F06E-9C46-4A44-AC32-4ED0C2CF8BC4}"/>
+    <hyperlink ref="C35" r:id="rId34" display="mailto:amelia.johnson88@protonmail.com" xr:uid="{4EA6D74B-6612-425B-960B-5C61FC15E2E6}"/>
+    <hyperlink ref="C36" r:id="rId35" display="mailto:mason.davis91@gmail.com" xr:uid="{C67E91C9-EAF1-4613-B55E-EB1BA772FEE7}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+</worksheet>
 </file>
</xml_diff>